<commit_message>
Added folders and some test examples
</commit_message>
<xml_diff>
--- a/Agile Project Charter.xlsx
+++ b/Agile Project Charter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Computing\Documents\ASE_Assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88511D85-564D-4C19-8671-FB9218F28FDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43273145-14D7-4272-99FB-389E274A53E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,9 +84,6 @@
     <t>Mitchell</t>
   </si>
   <si>
-    <t>Lecturers, Developers</t>
-  </si>
-  <si>
     <t>James Gibson</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>A robust back-end and a user-friendly interface. An application that meets all of the projects requirements</t>
+  </si>
+  <si>
+    <t>Lecturers, Project Team</t>
   </si>
 </sst>
 </file>
@@ -870,8 +870,8 @@
   <dimension ref="B1:M51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14:E14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -958,7 +958,7 @@
       </c>
       <c r="C5" s="38"/>
       <c r="D5" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>16</v>
@@ -990,7 +990,7 @@
     </row>
     <row r="7" spans="2:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="30" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="31"/>
@@ -1079,7 +1079,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="39"/>
       <c r="E12" s="40"/>
@@ -1097,7 +1097,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="18"/>

</xml_diff>

<commit_message>
Updated names on the project charter to be full names
</commit_message>
<xml_diff>
--- a/Agile Project Charter.xlsx
+++ b/Agile Project Charter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Computing\Documents\ASE_Assessment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\University\Advanced Software Engineering\ASE_Assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43273145-14D7-4272-99FB-389E274A53E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919AFF2C-3A44-4CCE-914F-FC02DA998A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Project Charter" sheetId="1" r:id="rId1"/>
@@ -78,12 +78,6 @@
     <t>We are risking the potetntial loss of money and time. We are also risking the loss of customers/money if the service has problems.</t>
   </si>
   <si>
-    <t>Michael</t>
-  </si>
-  <si>
-    <t>Mitchell</t>
-  </si>
-  <si>
     <t>James Gibson</t>
   </si>
   <si>
@@ -94,6 +88,12 @@
   </si>
   <si>
     <t>Lecturers, Project Team</t>
+  </si>
+  <si>
+    <t>Michael Edwards</t>
+  </si>
+  <si>
+    <t>Mitchell Seng</t>
   </si>
 </sst>
 </file>
@@ -395,7 +395,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -403,13 +403,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -418,19 +415,19 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -442,19 +439,19 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -484,13 +481,13 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -499,22 +496,22 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -871,7 +868,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7:E7"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -885,12 +882,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -901,12 +898,12 @@
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="2:13" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -917,12 +914,12 @@
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="2:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -933,14 +930,14 @@
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="36"/>
+      <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="1"/>
@@ -953,15 +950,15 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="2:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="37"/>
+      <c r="D5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>16</v>
+      <c r="E5" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -973,12 +970,12 @@
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -989,12 +986,12 @@
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="2:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
+      <c r="B7" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="31"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1005,14 +1002,14 @@
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="7" t="s">
+      <c r="C8" s="33"/>
+      <c r="D8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="1"/>
@@ -1025,14 +1022,14 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="2:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="35">
+      <c r="B9" s="34">
         <v>45343</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="16">
+      <c r="C9" s="35"/>
+      <c r="D9" s="15">
         <v>45421</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="11">
         <v>45372</v>
       </c>
       <c r="F9" s="1"/>
@@ -1045,10 +1042,10 @@
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="2:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1059,12 +1056,12 @@
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="2:13" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1075,14 +1072,14 @@
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="2:13" ht="144.94999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="40"/>
+      <c r="C12" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1093,14 +1090,14 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="2:13" ht="144.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="18"/>
+      <c r="C13" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1111,14 +1108,14 @@
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="2:13" ht="144.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>

</xml_diff>